<commit_message>
7/14 update When opening the DatePicker, there is not going to be any date selected if user did not pick one before.
</commit_message>
<xml_diff>
--- a/props.xlsx
+++ b/props.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20375"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pi\OneDrive\Desktop\Programming\react-native-date-picker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{60559D2A-803E-4ED2-8004-19489158AE2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AF3C77-2C17-4ED7-A88D-F56310CFAED0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17580" xr2:uid="{24858876-E1FF-4C8C-914A-B579E497A88E}"/>
   </bookViews>
@@ -25,28 +25,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>Attributes</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>value</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>discription</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>isVisible</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>setIsVisible</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>displayDate</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -95,10 +83,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>按下確定時要執行的動作</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>模式選擇，單日:'single' 多日: 'range'</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -107,7 +91,41 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>控制isVisible的函數</t>
+    <t>startDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>endDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>首次打開畫面時所選取的第一個日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Discription</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>首次打開畫面時所選取的最後一個日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>onCancel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>按下取消要執行的動作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>按下確定時要執行的動作 
+single: 傳入 date argument
+range: 傳入 startDate, endDate 兩個 argument</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -243,7 +261,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -279,6 +297,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -594,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CCA13EA-F405-4B9F-8CB0-DBDCE6B3AF40}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -612,98 +633,110 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>11</v>
+        <v>3</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>13</v>
+        <v>22</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>17</v>
+        <v>8</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="C7" s="10" t="s">
         <v>12</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C8" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="10"/>
+      <c r="B9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="10"/>
+      <c r="A10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
@@ -715,15 +748,10 @@
       <c r="B12" s="5"/>
       <c r="C12" s="10"/>
     </row>
-    <row r="13" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="10"/>
-    </row>
-    <row r="14" spans="1:3" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="11"/>
+    <row r="13" spans="1:3" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
7/18 colorOptions small update
</commit_message>
<xml_diff>
--- a/props.xlsx
+++ b/props.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pi\OneDrive\Desktop\Programming\react-native-date-picker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7FE349-1337-4617-9CAC-227BB4A203C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B66938-9A3D-42C8-A01B-C5C3BF914DFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17580" xr2:uid="{24858876-E1FF-4C8C-914A-B579E497A88E}"/>
   </bookViews>
@@ -161,24 +161,24 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>initialDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一次開啟視窗時，顯示這個日期所在的月份</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>控制元件各個部分的顏色
-dateTextColor,
-dateBackgroundColor,
-selectedDateColor,
-selectedDateBackgroundColor,
-headerColor,
-weekDaysColor,
-backgroundColor,
-confirmButtonColor,
-changeYearModalColor,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>initialDate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>第一次開啟視窗時，顯示這個日期所在的月份</t>
+backgroundColor: 整個元件的背景顏色，包括日期按鈕和切換年份視窗的背景
+headerColor: header 的背景顏色
+headerTextColor: header 的文字顏色和切換月份的 icon 顏色
+changeYearModalColor: 切換年份視窗的主色
+weekDaysColor: 星期文字的顏色
+dateTextColor: 日期按鈕中的文字顏色 (6碼HEX)
+selectedDateColor: 當日期按鈕被active 時的文字顏色 (6碼HEX)
+selectedDateBackgroundColor: 當日期按鈕被 active 時的背景顏色 (6碼HEX)
+confirmButtonColor: 確認按鈕的文字顏色</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -573,7 +573,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -640,13 +640,13 @@
     </row>
     <row r="6" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -734,7 +734,7 @@
         <v>28</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>